<commit_message>
Regular update on 6/25
</commit_message>
<xml_diff>
--- a/position.xlsx
+++ b/position.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gombae/Documents/invest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3F6D47-BB45-724B-BEA1-17C7C0F7AE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE638028-B9BD-F449-A431-9D31A877DA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="capital" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="ticker" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="133">
   <si>
     <t>2022-04-21</t>
   </si>
@@ -445,6 +446,46 @@
   </si>
   <si>
     <t>2022-06-01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>218420</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>KODEX 미국S&amp;P에너지(합성)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>500014</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>신한 인버스 옥수수 선물 ETN(H)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>500058</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>신한 S&amp;P500 VIX S/T 선물 ETN C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>510004</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대신 인버스 아연선물 ETN(H)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>510018</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대신 인버스 알루미늄 선물 ETN(H)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -454,7 +495,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -502,15 +543,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
@@ -863,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0227AC08-FF2A-5442-BE36-AE10F5ED8DF2}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -2425,10 +2467,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4758F4D2-842C-B340-A5AB-839768A9D55B}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -2718,19 +2760,19 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F13" t="s">
         <v>98</v>
@@ -2740,37 +2782,37 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="2">
-        <v>241180</v>
+      <c r="A14" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="F14" t="s">
         <v>98</v>
       </c>
       <c r="G14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2">
-        <v>256440</v>
+        <v>241180</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C15" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="D15" t="s">
         <v>92</v>
@@ -2786,20 +2828,20 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="2" t="s">
-        <v>22</v>
+      <c r="A16" s="2">
+        <v>256440</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F16" t="s">
         <v>98</v>
@@ -2809,17 +2851,17 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="2">
-        <v>269370</v>
+      <c r="A17" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
         <v>95</v>
@@ -2832,60 +2874,60 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="2">
+        <v>269370</v>
+      </c>
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>51</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>47</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>39</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>49</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>99</v>
       </c>
-      <c r="G18" t="b">
+      <c r="G19" t="b">
         <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="2">
-        <v>305540</v>
-      </c>
-      <c r="B19" t="s">
-        <v>104</v>
-      </c>
-      <c r="C19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" t="s">
-        <v>95</v>
-      </c>
-      <c r="F19" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2">
-        <v>309230</v>
+        <v>305540</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="D20" t="s">
         <v>92</v>
@@ -2901,20 +2943,20 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="2" t="s">
-        <v>16</v>
+      <c r="A21" s="2">
+        <v>309230</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>113</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="E21" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F21" t="s">
         <v>98</v>
@@ -2925,19 +2967,19 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
         <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="F22" t="s">
         <v>98</v>
@@ -2948,25 +2990,25 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D23" t="s">
         <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F23" t="s">
         <v>98</v>
       </c>
       <c r="G23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2994,42 +3036,42 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
         <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F25" t="s">
         <v>98</v>
       </c>
       <c r="G25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="2">
-        <v>367770</v>
+      <c r="A26" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="E26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F26" t="s">
         <v>98</v>
@@ -3039,17 +3081,17 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="2" t="s">
-        <v>24</v>
+      <c r="A27" s="2">
+        <v>367770</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="E27" t="s">
         <v>95</v>
@@ -3063,13 +3105,13 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D28" t="s">
         <v>39</v>
@@ -3085,46 +3127,46 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="2">
+      <c r="A29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="2">
         <v>373530</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>108</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>102</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>92</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>94</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>99</v>
-      </c>
-      <c r="G29" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" t="s">
-        <v>95</v>
-      </c>
-      <c r="F30" t="s">
-        <v>98</v>
       </c>
       <c r="G30" t="b">
         <v>1</v>
@@ -3132,13 +3174,13 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D31" t="s">
         <v>39</v>
@@ -3154,17 +3196,17 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="2">
-        <v>394670</v>
+      <c r="A32" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>110</v>
+        <v>47</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="E32" t="s">
         <v>95</v>
@@ -3177,23 +3219,23 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="2" t="s">
-        <v>13</v>
+      <c r="A33" s="2">
+        <v>394670</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="D33" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G33" t="b">
         <v>1</v>
@@ -3201,10 +3243,10 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
         <v>43</v>
@@ -3213,79 +3255,79 @@
         <v>39</v>
       </c>
       <c r="E34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" t="s">
+        <v>99</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" t="s">
         <v>95</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F35" t="s">
         <v>98</v>
       </c>
-      <c r="G34" t="b">
+      <c r="G35" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="2">
+    <row r="36" spans="1:7">
+      <c r="A36" s="2">
         <v>500058</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>87</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>88</v>
-      </c>
-      <c r="D35" t="s">
-        <v>91</v>
-      </c>
-      <c r="E35" t="s">
-        <v>94</v>
-      </c>
-      <c r="F35" t="s">
-        <v>100</v>
-      </c>
-      <c r="G35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" t="s">
-        <v>47</v>
       </c>
       <c r="D36" t="s">
         <v>91</v>
       </c>
       <c r="E36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F36" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="2" t="s">
-        <v>9</v>
+      <c r="A37" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="C37" t="s">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="D37" t="s">
         <v>91</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G37" t="b">
         <v>1</v>
@@ -3293,13 +3335,13 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="2" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="D38" t="s">
         <v>91</v>
@@ -3316,37 +3358,152 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" t="s">
-        <v>68</v>
+        <v>129</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="C39" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="D39" t="s">
         <v>91</v>
       </c>
       <c r="E39" t="s">
+        <v>96</v>
+      </c>
+      <c r="F39" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" t="s">
+        <v>96</v>
+      </c>
+      <c r="F40" t="s">
+        <v>99</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" t="s">
+        <v>96</v>
+      </c>
+      <c r="F41" t="s">
+        <v>99</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" t="s">
         <v>95</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F42" t="s">
         <v>98</v>
       </c>
-      <c r="G39" t="b">
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" t="s">
+        <v>94</v>
+      </c>
+      <c r="F43" t="s">
+        <v>100</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" t="s">
+        <v>95</v>
+      </c>
+      <c r="F44" t="s">
+        <v>98</v>
+      </c>
+      <c r="G44" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G2:G39">
+  <conditionalFormatting sqref="G2:G44">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A36:A39 A2:A11 A16 A13 A18 A30:A31 A27:A28 A21:A25 A33:A34" numberStoredAsText="1"/>
+    <ignoredError sqref="A42:A44 A2:A11 A17 A14 A19 A31:A32 A28:A29 A34:A35 A22:A23 A25:A26 A40" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>